<commit_message>
university conditional statements updated
</commit_message>
<xml_diff>
--- a/documents/questionchecklist_202101280200.xlsx
+++ b/documents/questionchecklist_202101280200.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Patrick\HKUSpace\FYP\Asso-yr2-FYP\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62477012-FF78-47BF-97E9-0769621617E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E09438E-D3F2-4DC7-B2B2-3E0CB4BE4180}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1440" windowWidth="29040" windowHeight="16440" xr2:uid="{4A17C007-98B6-4593-9A05-559A17A03F10}"/>
+    <workbookView xWindow="34308" yWindow="10512" windowWidth="21600" windowHeight="11772" xr2:uid="{4A17C007-98B6-4593-9A05-559A17A03F10}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -65,555 +65,558 @@
     <t>What is Non-JUPAS?</t>
   </si>
   <si>
+    <t>NONJUPAS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text Only</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youth.gov.hk/en/career-and-study/stories/detail.htm?content-id=2385436&amp;section=CSA</t>
+  </si>
+  <si>
+    <t>When can I apply for Non-JUPAS application?</t>
+  </si>
+  <si>
+    <t>Which university you want to apply?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the deadline of Non-JUPAS application?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Each university may vary.</t>
+  </si>
+  <si>
+    <t>Which university you want to apply/ have applied?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What do I need to prepare for Non-JUPAS application?</t>
+  </si>
+  <si>
+    <t>Each university may vary. But Generally, you should better prepare your personal identify information(e.g. HKID / Passport / etc), public examination results(e.g. HKDSE / HKCEE /HKALE / IGCSE / IELTS / TOFEL / etc), official transcript, personal statement, other appropriate qualification documents (e.g. public non-academic awards / etc),  etc.</t>
+  </si>
+  <si>
+    <t>Can I apply for Non-JUPAS application in AD/HD Year1?</t>
+  </si>
+  <si>
+    <t>You can apply non-jupas application when you are year 1 student,  but bare in mind that some universities may only consider senior level student and some might only consider junior level student.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will the School provide any support for us upon the application? e.g. collecting all the applications and send to the university</t>
+  </si>
+  <si>
+    <t>Text + http</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the standard requirement for Non-JUPAS applications?</t>
+  </si>
+  <si>
+    <t>It depends on the university you want to apply and the programme you want to apply. For general requirement in applying the universities in Hong Kong, you should as least have GRADE 3 for both Chinese and English language subject and 5 subjects in GRADE 2 for HKDSE result. For the language subject, you can use the result of IELTS and IGCSE instead but the requirement for each univerisity and programme may vary.</t>
+  </si>
+  <si>
+    <t>Which programe and university you want to apply/ have applied?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can I apply for more than one application at the same time?</t>
+  </si>
+  <si>
+    <t>Each university may vary.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I cannot submit the application on time, what should I do?</t>
+  </si>
+  <si>
+    <t>Indeed, late submission would not be allowed. Although the univerisities usually have many rounds of non-JUPAS application, it is recommend to submit the application as soon as possible. You may contact to their admission office directly if you want some help.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is it a must to have a reference letter for Non-JUPAS application?</t>
+  </si>
+  <si>
+    <t>Indeed. the associate programme is aimed to assist the students to promote their academic position to undergraduate level but not for profession purpose. Students are supposed to apply NON-JUPAS before they are graduated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to apply  non-jupas ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can apply the non-jupas from any University's non-jupas page. </t>
+  </si>
+  <si>
+    <t>how to apply university through non-jupas ?</t>
+  </si>
+  <si>
+    <t>How to apply financial support (in HKUspace) ? </t>
+  </si>
+  <si>
+    <t>FINANCE</t>
+  </si>
+  <si>
+    <t>Any link yo the financial support page ? </t>
+  </si>
+  <si>
+    <t>What is the deadline of applying financial support ? </t>
+  </si>
+  <si>
+    <t>What should I do to apply financial support ? </t>
+  </si>
+  <si>
+    <t>What I have to do to apply financial support ? </t>
+  </si>
+  <si>
+    <t>Where can I get my financial support ? </t>
+  </si>
+  <si>
+    <t>Who can I submit to after finishing my financial support form ? </t>
+  </si>
+  <si>
+    <t>Does the quantity of reference letter matter?</t>
+  </si>
+  <si>
+    <t>Each university and programme may vary.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can I apply IGCSE English instead of IELTS for English qualification?</t>
+  </si>
+  <si>
+    <t>What can I apply in the School?</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What can I do if I want to change the personal information?</t>
+  </si>
+  <si>
+    <t>When will be the class add/drop/swap period?</t>
+  </si>
+  <si>
+    <t>What can I do if I want to swap class with my classmate?</t>
+  </si>
+  <si>
+    <t>Can I swap the classes between semesters?</t>
+  </si>
+  <si>
+    <t>Where can I find the course outline before taking the course?</t>
+  </si>
+  <si>
+    <t>I accidentally dropped a mandatory course and cannot add it back during the add/drop period. What can I do?</t>
+  </si>
+  <si>
+    <t>After studying for couple weeks, I think the course does not suit me. Can I change it now?</t>
+  </si>
+  <si>
+    <t>What can I do if I believe that my academic result is not assessed probably? Does appeal really help?</t>
+  </si>
+  <si>
+    <t>When can I start to apply for the result appeal?</t>
+  </si>
+  <si>
+    <t>How long does it take for the feedback of result appeal?</t>
+  </si>
+  <si>
+    <t>I lost my student ID/HKU facility Card. What should I do?</t>
+  </si>
+  <si>
+    <t>After studying for one semester, I think this programme does not suit me. Can I change it now?</t>
+  </si>
+  <si>
+    <t>I accidentally receive the bachelor degree offer after tuition fee payment. Can I get back a refund?</t>
+  </si>
+  <si>
+    <t>How can I know the time schedule and who will be the lecturer teaching for specific class?</t>
+  </si>
+  <si>
+    <t>How can I get access to the master timetable for the coming semester?</t>
+  </si>
+  <si>
+    <t>What should I do if I want to defer the tuition fee payment deadline?</t>
+  </si>
+  <si>
+    <t>I cannot login to my learner portal/SCORE/SOUL/student-Gmail account . What can I do?</t>
+  </si>
+  <si>
+    <t>ONLINE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>My learner portal/SCORE/SOUL account has been locked by the system. What can I do?</t>
+  </si>
+  <si>
+    <t>[SOUL]I could not find my registered course in SOUL. What should I do?</t>
+  </si>
+  <si>
+    <t>[SOUL]I could not upload my file for submission. What should I do?</t>
+  </si>
+  <si>
+    <t>[SOUL]Can I modify the submitted file before the deadline? How?</t>
+  </si>
+  <si>
+    <t>[SOUL]I could not submit the assignment on time. What should I do?</t>
+  </si>
+  <si>
+    <t>[SCORE]How can I find my unofficial transcript through the online platform?</t>
+  </si>
+  <si>
+    <t>[Learner Portal]How can I pay the tuition fee online?</t>
+  </si>
+  <si>
+    <t>Is there any scholarship(s) or financial reimbursement to apply?</t>
+  </si>
+  <si>
+    <t>FINANCE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What should I do if I want to apply for Student Octopus?</t>
+  </si>
+  <si>
+    <t>You can give a fully-filled student octupos application form to general office. After processing, you can collect back the form and submit to the "Student Octopus Application Form Collect Box" available in the MTR station.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Which one is your main campus?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Where is the [FACILITY] ?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FACILITY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Where is the [FACILITY] in [CAMPUS]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[FACILITY] is/are in [FLOOR ROOM].</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What facilites does the [CAMPUS] have?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[CAMPUS] has [FACILITIES]. {[FACILITY A] is in [FLOOR ROOM]. [FACILITY B] is in [FLOOR ROOM]. ...}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the contact of [OFFICE] in [CAMPUS]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The contact is [TELE]. the office hour is {[OFFICE HOURS]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does [CAMPUS] have [FACILITY]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes, [FACILITY] is/are in [FLOOR ROOM]. / No, [CAMPUS] does not have [FACILITY].</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the open hour of the [FACILITY]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the open hour of the [FACILITY] in [CAMPUS]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The opening hour is {[OPENING HOURS]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is [FACILITY] opening now?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is [FACILITY] in [CAMPUS] opening now?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes, [FACILITY] is/are available until [NEXT CLOSE TIME]. / No, [CAMPUS] does not have [FACILITY]. / No, [FACILITY] will be open at [NEXT OPEN TIME].</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to get in [UNIVERSITY] ?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the non-jupas deadline of [UNIVERSITY] ? </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the deadline of  [UNIVERSITY] ? </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do you mean non-JUPAS deadline?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y/N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any link to [UNIVERSITY] ?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Which university are you refering to?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[UNIVERSITY] have [NUM] round(s) non-JUPAS application. They are as the following: {[ROUND DEADLINE]} </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GREETING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[GREETING]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[CLOSING]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[GREETINGS]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[CLOSINGS]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>contact</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>greeting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>closing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any link to the non-jupas page? </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">You can apply the non-jupas from [UNIVERSITY] non-jupas page. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKUSPACE have setup an online platform in learner portal for student to apply for the reference letter from the professor. Make sure you have get the professor's approval before apply for the letter through the online platform. You may refer to [HTTP] for further information</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text + Hyperlink</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>partially implemented</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whatis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whenis_open_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whenis_deadline_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>what_toprepare_general</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_apply_year1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>schoolsupport_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whatis_requirement_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_apply_morethan1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>action_latetosubmit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_essential_referenceletter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is it a must for year-2 AD student to apply senior year Non-JUPAS application?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_essential_apply_year2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Do you mean the webpage of [UNIVERSITY]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name: university value: [UNIVERSITY]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>howto_webpage_university</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>howto_apply_university</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whenis_deadline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonjupas_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">You can apply the non-JUPAS from the University's webpage. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_num_referenceletter_matter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>When will the application of [PUBLICEXAM] start?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>When can I apply the [PUBLICEXAM]?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whenis_start_publicexam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name: exam value: [PUBLICEXAM]</t>
+  </si>
+  <si>
+    <t>name: exam value: [PUBLICEXAM]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>whencan_apply_publicexam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>You can apply it before [DEADLINE] / at anytime. Please refer to [HTTP] for more information.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>You may refer to [HTTP] for more information.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_igcse_replace_ielts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>location_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name: campus, value: [CAMPUS]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name: office, value: [FACILITY]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name: facility, value: [FACILITY]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>campus_have</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>openinghour_facility</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>openinghour_facility_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name: facility, value: [FACILITY], name: campus, value: [CAMPUS]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>campus_have_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_facility_open_nospecific</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yn_facility_open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>howto_webpage_university</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Apart from getting a place into universities through JUPAS, students may consider applying post-secondary programmes not covered by JUPAS. There is a lot of information regarding non-JUPAS admissions. Gather your information in advance and plan ahead.</t>
-  </si>
-  <si>
-    <t>NONJUPAS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Text Only</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.youth.gov.hk/en/career-and-study/stories/detail.htm?content-id=2385436&amp;section=CSA</t>
-  </si>
-  <si>
-    <t>When can I apply for Non-JUPAS application?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>You can apply non-jupas application once it is open. Each university may vary.</t>
-  </si>
-  <si>
-    <t>Which university you want to apply?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the deadline of Non-JUPAS application?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Each university may vary.</t>
-  </si>
-  <si>
-    <t>Which university you want to apply/ have applied?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What do I need to prepare for Non-JUPAS application?</t>
-  </si>
-  <si>
-    <t>Each university may vary. But Generally, you should better prepare your personal identify information(e.g. HKID / Passport / etc), public examination results(e.g. HKDSE / HKCEE /HKALE / IGCSE / IELTS / TOFEL / etc), official transcript, personal statement, other appropriate qualification documents (e.g. public non-academic awards / etc),  etc.</t>
-  </si>
-  <si>
-    <t>Can I apply for Non-JUPAS application in AD/HD Year1?</t>
-  </si>
-  <si>
-    <t>You can apply non-jupas application when you are year 1 student,  but bare in mind that some universities may only consider senior level student and some might only consider junior level student.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Will the School provide any support for us upon the application? e.g. collecting all the applications and send to the university</t>
-  </si>
-  <si>
-    <t>Text + http</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the standard requirement for Non-JUPAS applications?</t>
-  </si>
-  <si>
-    <t>It depends on the university you want to apply and the programme you want to apply. For general requirement in applying the universities in Hong Kong, you should as least have GRADE 3 for both Chinese and English language subject and 5 subjects in GRADE 2 for HKDSE result. For the language subject, you can use the result of IELTS and IGCSE instead but the requirement for each univerisity and programme may vary.</t>
-  </si>
-  <si>
-    <t>Which programe and university you want to apply/ have applied?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can I apply for more than one application at the same time?</t>
-  </si>
-  <si>
-    <t>Each university may vary.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>I cannot submit the application on time, what should I do?</t>
-  </si>
-  <si>
-    <t>Indeed, late submission would not be allowed. Although the univerisities usually have many rounds of non-JUPAS application, it is recommend to submit the application as soon as possible. You may contact to their admission office directly if you want some help.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is it a must to have a reference letter for Non-JUPAS application?</t>
-  </si>
-  <si>
-    <t>Indeed. the associate programme is aimed to assist the students to promote their academic position to undergraduate level but not for profession purpose. Students are supposed to apply NON-JUPAS before they are graduated</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>How to apply  non-jupas ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can apply the non-jupas from any University's non-jupas page. </t>
-  </si>
-  <si>
-    <t>how to apply university through non-jupas ?</t>
-  </si>
-  <si>
-    <t>How to apply financial support (in HKUspace) ? </t>
-  </si>
-  <si>
-    <t>FINANCE</t>
-  </si>
-  <si>
-    <t>Any link yo the financial support page ? </t>
-  </si>
-  <si>
-    <t>What is the deadline of applying financial support ? </t>
-  </si>
-  <si>
-    <t>What should I do to apply financial support ? </t>
-  </si>
-  <si>
-    <t>What I have to do to apply financial support ? </t>
-  </si>
-  <si>
-    <t>Where can I get my financial support ? </t>
-  </si>
-  <si>
-    <t>Who can I submit to after finishing my financial support form ? </t>
-  </si>
-  <si>
-    <t>Does the quantity of reference letter matter?</t>
-  </si>
-  <si>
-    <t>Each university and programme may vary.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can I apply IGCSE English instead of IELTS for English qualification?</t>
-  </si>
-  <si>
-    <t>What can I apply in the School?</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What can I do if I want to change the personal information?</t>
-  </si>
-  <si>
-    <t>When will be the class add/drop/swap period?</t>
-  </si>
-  <si>
-    <t>What can I do if I want to swap class with my classmate?</t>
-  </si>
-  <si>
-    <t>Can I swap the classes between semesters?</t>
-  </si>
-  <si>
-    <t>Where can I find the course outline before taking the course?</t>
-  </si>
-  <si>
-    <t>I accidentally dropped a mandatory course and cannot add it back during the add/drop period. What can I do?</t>
-  </si>
-  <si>
-    <t>After studying for couple weeks, I think the course does not suit me. Can I change it now?</t>
-  </si>
-  <si>
-    <t>What can I do if I believe that my academic result is not assessed probably? Does appeal really help?</t>
-  </si>
-  <si>
-    <t>When can I start to apply for the result appeal?</t>
-  </si>
-  <si>
-    <t>How long does it take for the feedback of result appeal?</t>
-  </si>
-  <si>
-    <t>I lost my student ID/HKU facility Card. What should I do?</t>
-  </si>
-  <si>
-    <t>After studying for one semester, I think this programme does not suit me. Can I change it now?</t>
-  </si>
-  <si>
-    <t>I accidentally receive the bachelor degree offer after tuition fee payment. Can I get back a refund?</t>
-  </si>
-  <si>
-    <t>How can I know the time schedule and who will be the lecturer teaching for specific class?</t>
-  </si>
-  <si>
-    <t>How can I get access to the master timetable for the coming semester?</t>
-  </si>
-  <si>
-    <t>What should I do if I want to defer the tuition fee payment deadline?</t>
-  </si>
-  <si>
-    <t>I cannot login to my learner portal/SCORE/SOUL/student-Gmail account . What can I do?</t>
-  </si>
-  <si>
-    <t>ONLINE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>My learner portal/SCORE/SOUL account has been locked by the system. What can I do?</t>
-  </si>
-  <si>
-    <t>[SOUL]I could not find my registered course in SOUL. What should I do?</t>
-  </si>
-  <si>
-    <t>[SOUL]I could not upload my file for submission. What should I do?</t>
-  </si>
-  <si>
-    <t>[SOUL]Can I modify the submitted file before the deadline? How?</t>
-  </si>
-  <si>
-    <t>[SOUL]I could not submit the assignment on time. What should I do?</t>
-  </si>
-  <si>
-    <t>[SCORE]How can I find my unofficial transcript through the online platform?</t>
-  </si>
-  <si>
-    <t>[Learner Portal]How can I pay the tuition fee online?</t>
-  </si>
-  <si>
-    <t>Is there any scholarship(s) or financial reimbursement to apply?</t>
-  </si>
-  <si>
-    <t>FINANCE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What should I do if I want to apply for Student Octopus?</t>
-  </si>
-  <si>
-    <t>You can give a fully-filled student octupos application form to general office. After processing, you can collect back the form and submit to the "Student Octopus Application Form Collect Box" available in the MTR station.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Which one is your main campus?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Where is the [FACILITY] ?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FACILITY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Where is the [FACILITY] in [CAMPUS]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[FACILITY] is/are in [FLOOR ROOM].</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What facilites does the [CAMPUS] have?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[CAMPUS] has [FACILITIES]. {[FACILITY A] is in [FLOOR ROOM]. [FACILITY B] is in [FLOOR ROOM]. ...}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the contact of [OFFICE] in [CAMPUS]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The contact is [TELE]. the office hour is {[OFFICE HOURS]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Does [CAMPUS] have [FACILITY]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes, [FACILITY] is/are in [FLOOR ROOM]. / No, [CAMPUS] does not have [FACILITY].</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the open hour of the [FACILITY]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the open hour of the [FACILITY] in [CAMPUS]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The opening hour is {[OPENING HOURS]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is [FACILITY] opening now?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is [FACILITY] in [CAMPUS] opening now?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes, [FACILITY] is/are available until [NEXT CLOSE TIME]. / No, [CAMPUS] does not have [FACILITY]. / No, [FACILITY] will be open at [NEXT OPEN TIME].</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modifier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>How to get in [UNIVERSITY] ?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the non-jupas deadline of [UNIVERSITY] ? </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>What is the deadline of  [UNIVERSITY] ? </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Do you mean non-JUPAS deadline?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y/N</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Any link to [UNIVERSITY] ?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Which university are you refering to?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[UNIVERSITY] have [NUM] round(s) non-JUPAS application. They are as the following: {[ROUND DEADLINE]} </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GREETING</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[GREETING]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[CLOSING]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[GREETINGS]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[CLOSINGS]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>contact</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>greeting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>closing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Any link to the non-jupas page? </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">You can apply the non-jupas from [UNIVERSITY] non-jupas page. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HKUSPACE have setup an online platform in learner portal for student to apply for the reference letter from the professor. Make sure you have get the professor's approval before apply for the letter through the online platform. You may refer to [HTTP] for further information</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Text + Hyperlink</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>partially implemented</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whatis</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whenis_open_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whenis_deadline_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>what_toprepare_general</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_apply_year1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>schoolsupport_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whatis_requirement_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_apply_morethan1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>action_latetosubmit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_essential_referenceletter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Is it a must for year-2 AD student to apply senior year Non-JUPAS application?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_essential_apply_year2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Do you mean the webpage of [UNIVERSITY]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name: university value: [UNIVERSITY]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>howto_webpage_university</t>
-  </si>
-  <si>
-    <t>howto_webpage_university</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>howto_apply_university</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whenis_deadline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonjupas_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">You can apply the non-JUPAS from the University's webpage. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_num_referenceletter_matter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>When will the application of [PUBLICEXAM] start?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>When can I apply the [PUBLICEXAM]?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whenis_start_publicexam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name: exam value: [PUBLICEXAM]</t>
-  </si>
-  <si>
-    <t>name: exam value: [PUBLICEXAM]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>whencan_apply_publicexam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>You can apply it before [DEADLINE] / at anytime. Please refer to [HTTP] for more information.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>You may refer to [HTTP] for more information.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_igcse_replace_ielts</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>location_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>location</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{name: campus, value: [CAMPUS]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{name: office, value: [FACILITY]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{name: facility, value: [FACILITY]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>campus_have</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>openinghour_facility</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>openinghour_facility_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{name: facility, value: [FACILITY], name: campus, value: [CAMPUS]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>campus_have_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_facility_open_nospecific</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yn_facility_open</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1012,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7748AE44-D27D-44E6-AE9F-E6FAF9B675AC}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1049,10 +1052,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1078,19 +1081,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1098,22 +1101,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1121,22 +1124,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1144,22 +1147,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1167,22 +1170,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1190,19 +1193,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1210,22 +1213,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1233,22 +1236,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1256,22 +1259,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1279,22 +1282,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1302,19 +1305,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1322,25 +1325,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1348,19 +1351,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1368,19 +1371,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1388,19 +1391,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1408,25 +1411,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" t="s">
         <v>102</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>103</v>
-      </c>
-      <c r="J17" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1434,22 +1437,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1457,22 +1460,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1480,22 +1483,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1503,22 +1506,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1526,22 +1529,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1549,22 +1552,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1572,10 +1575,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1583,10 +1586,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1594,10 +1597,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1605,10 +1608,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1616,10 +1619,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1627,10 +1630,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1638,10 +1641,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1649,10 +1652,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1660,10 +1663,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1671,10 +1674,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1682,10 +1685,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1693,10 +1696,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1704,10 +1707,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1715,10 +1718,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1726,10 +1729,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1737,10 +1740,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1748,10 +1751,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1759,10 +1762,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1770,10 +1773,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,10 +1784,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1792,10 +1795,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1803,10 +1806,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1814,10 +1817,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1825,10 +1828,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1836,10 +1839,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -1847,13 +1850,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -1861,19 +1864,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" t="s">
+        <v>76</v>
+      </c>
+      <c r="H50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" t="s">
         <v>79</v>
-      </c>
-      <c r="C50" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" t="s">
-        <v>78</v>
-      </c>
-      <c r="H50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -1881,10 +1884,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -1892,10 +1895,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -1903,10 +1906,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E53" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -1914,10 +1917,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -1925,10 +1928,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -1936,10 +1939,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E56" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -1947,10 +1950,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E57" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -1958,22 +1961,22 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E58" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -1981,25 +1984,25 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E59" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F59" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G59" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2007,22 +2010,22 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E60" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -2030,25 +2033,25 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G61" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -2056,22 +2059,22 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E62" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F62" t="s">
+        <v>153</v>
+      </c>
+      <c r="G62" t="s">
         <v>156</v>
       </c>
-      <c r="G62" t="s">
-        <v>159</v>
-      </c>
       <c r="H62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -2079,22 +2082,22 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E63" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F63" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G63" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I63" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -2102,22 +2105,22 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E64" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F64" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G64" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -2125,22 +2128,22 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E65" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F65" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G65" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -2148,22 +2151,22 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E66" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F66" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G66" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -2171,19 +2174,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" t="s">
         <v>109</v>
       </c>
-      <c r="C67" t="s">
-        <v>111</v>
-      </c>
       <c r="E67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F67" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -2191,19 +2194,19 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" t="s">
         <v>110</v>
       </c>
-      <c r="C68" t="s">
-        <v>112</v>
-      </c>
       <c r="E68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F68" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
facility conditional tree updated
</commit_message>
<xml_diff>
--- a/documents/questionchecklist_202101280200.xlsx
+++ b/documents/questionchecklist_202101280200.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Patrick\HKUSpace\FYP\Asso-yr2-FYP\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E09438E-D3F2-4DC7-B2B2-3E0CB4BE4180}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6912427F-4CB5-4F94-BE72-02CA82A8CBEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34308" yWindow="10512" windowWidth="21600" windowHeight="11772" xr2:uid="{4A17C007-98B6-4593-9A05-559A17A03F10}"/>
+    <workbookView xWindow="13020" yWindow="14808" windowWidth="21600" windowHeight="11772" xr2:uid="{4A17C007-98B6-4593-9A05-559A17A03F10}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="164">
   <si>
     <t>Index</t>
   </si>
@@ -617,6 +617,10 @@
   </si>
   <si>
     <t>You can apply non-jupas application once it is open. Each university may vary.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name: office, value: [FACILITY]}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1015,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7748AE44-D27D-44E6-AE9F-E6FAF9B675AC}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1969,6 +1973,9 @@
       <c r="F58" t="s">
         <v>148</v>
       </c>
+      <c r="G58" t="s">
+        <v>163</v>
+      </c>
       <c r="H58" t="s">
         <v>12</v>
       </c>

</xml_diff>